<commit_message>
Implemented get_matricule for leaves
</commit_message>
<xml_diff>
--- a/recipients.xlsx
+++ b/recipients.xlsx
@@ -58,7 +58,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -72,6 +72,13 @@
     </fill>
   </fills>
   <borders count="3">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -94,29 +101,22 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -446,7 +446,7 @@
     <col min="5" max="5" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -466,7 +466,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="4">
-        <v>30030654</v>
+        <v>30046391</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>4</v>
@@ -483,7 +483,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="4">
-        <v>30030721</v>
+        <v>30046179</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>6</v>
@@ -500,7 +500,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="4">
-        <v>30030722</v>
+        <v>30046112</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>4</v>
@@ -512,12 +512,12 @@
         <v>2024</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="20.25">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="2">
         <v>3</v>
       </c>
       <c r="B5" s="4">
-        <v>30030832</v>
+        <v>30045885</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>6</v>

</xml_diff>